<commit_message>
fixing indexing bug and adding a new test case for ColorFormat
</commit_message>
<xml_diff>
--- a/src/test/resources/test_files/originals/valid_input.xlsx
+++ b/src/test/resources/test_files/originals/valid_input.xlsx
@@ -1,74 +1,117 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28724"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://airarabia-my.sharepoint.com/personal/malhaq_isa_ae1/Documents/Desktop/ExcelColumnConvert/src/test/resources/test_files/originals/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://airarabia-my.sharepoint.com/personal/malhaq_isa_ae1/Documents/Documents/ExcelColumnConvert/ExcelColumnConvert/src/test/resources/test_files/originals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="11_74AC4085E3F66FFC05FC9890E22D62B1D0368FFE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B212923B-FE4E-4786-80E3-2668B6ECD460}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_74AC4085E3F66FFC05FC9890E22D62B1D0368FFE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BB237DB-99F4-47B5-8B5E-7D7B3DEF86B1}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="28800" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="23">
   <si>
     <t>10</t>
   </si>
   <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>text1</t>
+  </si>
+  <si>
     <t>20</t>
   </si>
   <si>
+    <t>6.6</t>
+  </si>
+  <si>
+    <t>text2</t>
+  </si>
+  <si>
     <t>30</t>
   </si>
   <si>
+    <t>7.7</t>
+  </si>
+  <si>
+    <t>text3</t>
+  </si>
+  <si>
     <t>40</t>
   </si>
   <si>
+    <t>8.8</t>
+  </si>
+  <si>
+    <t>text4</t>
+  </si>
+  <si>
     <t>50</t>
   </si>
   <si>
-    <t>5.5</t>
-  </si>
-  <si>
-    <t>6.6</t>
-  </si>
-  <si>
-    <t>7.7</t>
-  </si>
-  <si>
-    <t>8.8</t>
-  </si>
-  <si>
     <t>9.9</t>
   </si>
   <si>
-    <t>text1</t>
-  </si>
-  <si>
-    <t>text2</t>
-  </si>
-  <si>
-    <t>text3</t>
-  </si>
-  <si>
-    <t>text4</t>
+    <t>5.6</t>
+  </si>
+  <si>
+    <t>6.7</t>
+  </si>
+  <si>
+    <t>7.8</t>
+  </si>
+  <si>
+    <t>8.9</t>
+  </si>
+  <si>
+    <t>9.10</t>
+  </si>
+  <si>
+    <t>5.7</t>
+  </si>
+  <si>
+    <t>6.8</t>
+  </si>
+  <si>
+    <t>7.9</t>
+  </si>
+  <si>
+    <t>8.10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,10 +163,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -413,15 +452,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -429,35 +468,35 @@
         <v>100</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D1">
         <v>1.1000000000000001</v>
       </c>
       <c r="E1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>200</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>2.2000000000000002</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>300</v>
@@ -469,44 +508,44 @@
         <v>3.3</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B4">
         <v>200</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D4">
         <v>4.4000000000000004</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>500</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D5">
         <v>5.5</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -514,35 +553,35 @@
         <v>100</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>1.1000000000000001</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B7">
         <v>200</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D7">
         <v>2.2000000000000002</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>300</v>
@@ -554,44 +593,44 @@
         <v>3.3</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>200</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D9">
         <v>4.4000000000000004</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>500</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D10">
         <v>5.5</v>
       </c>
       <c r="E10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -599,35 +638,35 @@
         <v>100</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <v>1.1000000000000001</v>
       </c>
       <c r="E11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B12">
         <v>200</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D12">
         <v>2.2000000000000002</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B13">
         <v>300</v>
@@ -639,41 +678,364 @@
         <v>3.3</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B14">
         <v>200</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D14">
         <v>4.4000000000000004</v>
       </c>
       <c r="E14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>500</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D15">
         <v>5.5</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>328.57142857142901</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>4.2428571428571402</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>337.142857142857</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>4.3607142857142902</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <v>345.71428571428601</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <v>4.4785714285714304</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>354.28571428571399</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19">
+        <v>4.5964285714285698</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20">
+        <v>362.857142857143</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20">
+        <v>4.71428571428571</v>
+      </c>
+      <c r="E20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>371.42857142857099</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21">
+        <v>4.83214285714286</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>380</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22">
+        <v>4.95</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>388.57142857142901</v>
+      </c>
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23">
+        <v>5.0678571428571404</v>
+      </c>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24">
+        <v>397.142857142857</v>
+      </c>
+      <c r="C24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24">
+        <v>5.1857142857142904</v>
+      </c>
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25">
+        <v>405.71428571428601</v>
+      </c>
+      <c r="C25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25">
+        <v>5.3035714285714297</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>414.28571428571399</v>
+      </c>
+      <c r="C26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26">
+        <v>5.4214285714285699</v>
+      </c>
+      <c r="E26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <v>422.857142857143</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27">
+        <v>5.5392857142857101</v>
+      </c>
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28">
+        <v>431.42857142857099</v>
+      </c>
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28">
+        <v>5.6571428571428601</v>
+      </c>
+      <c r="E28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29">
+        <v>440</v>
+      </c>
+      <c r="C29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29">
+        <v>5.7750000000000004</v>
+      </c>
+      <c r="E29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30">
+        <v>448.57142857142799</v>
+      </c>
+      <c r="C30" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30">
+        <v>5.8928571428571397</v>
+      </c>
+      <c r="E30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>457.142857142857</v>
+      </c>
+      <c r="C31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31">
+        <v>6.0107142857142897</v>
+      </c>
+      <c r="E31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32">
+        <v>465.71428571428601</v>
+      </c>
+      <c r="C32" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32">
+        <v>6.1285714285714299</v>
+      </c>
+      <c r="E32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <v>474.28571428571399</v>
+      </c>
+      <c r="C33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33">
+        <v>6.2464285714285701</v>
+      </c>
+      <c r="E33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34">
+        <v>482.857142857143</v>
+      </c>
+      <c r="C34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34">
+        <v>6.3642857142857103</v>
+      </c>
+      <c r="E34" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>